<commit_message>
added error analysis work.
</commit_message>
<xml_diff>
--- a/motif_analysis/test_results/worksheet.xlsx
+++ b/motif_analysis/test_results/worksheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Research\sequence-processing\motif_analysis\test_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Workspace\research\sequence-processing\motif_analysis\test_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44183CC-F584-4264-ABD5-8ECFCB288D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7811F412-22A8-4743-83AE-211FDDF85DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C9D092CA-C938-46FE-8B72-4B9A0C43BD65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C9D092CA-C938-46FE-8B72-4B9A0C43BD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="107">
   <si>
     <t>sequence</t>
   </si>
@@ -382,12 +382,72 @@
   <si>
     <t>TTTACAGGTATGCTC</t>
   </si>
+  <si>
+    <t xml:space="preserve">GAGATCGTCTCAGGT </t>
+  </si>
+  <si>
+    <t>training data</t>
+  </si>
+  <si>
+    <t>test data</t>
+  </si>
+  <si>
+    <t>predictions</t>
+  </si>
+  <si>
+    <r>
+      <t>ii</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ii</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>EEEEEEEEEii</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CA</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ATCGGCCCGGT</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +476,19 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -437,12 +510,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD3CEE9-AE39-4FAA-9079-FAABFEA4B360}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,20 +844,27 @@
     <col min="5" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>96</v>
       </c>
       <c r="E1" t="s">
         <v>97</v>
       </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,11 +883,16 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -826,8 +912,12 @@
         <v>49</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -836,7 +926,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -847,8 +937,12 @@
       <c r="G4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -857,7 +951,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -868,8 +962,11 @@
         <v>51</v>
       </c>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
@@ -880,6 +977,9 @@
         <v>52</v>
       </c>
       <c r="I6" s="1"/>
+      <c r="J6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>